<commit_message>
generación de json para actividad
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -453,12 +453,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Juan Carlos Presiga</t>
+          <t>Juan Carlos Presiga Montoya</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Infraestructura de Big_data</t>
+          <t>Infraestructura de Big_data Actividad 1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">

</xml_diff>